<commit_message>
add three graph(with bug)
</commit_message>
<xml_diff>
--- a/data/测试数据.xlsx
+++ b/data/测试数据.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD36148-20A1-406F-B07F-951A4A035686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="饼图" sheetId="1" r:id="rId1"/>
     <sheet name="折线图" sheetId="2" r:id="rId2"/>
     <sheet name="柱状图" sheetId="3" r:id="rId3"/>
+    <sheet name="仪表盘" sheetId="4" r:id="rId4"/>
+    <sheet name="漏斗图" sheetId="5" r:id="rId5"/>
+    <sheet name="雷达图" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>吃饭</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,11 +38,67 @@
     <t>时间占比</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>完成率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>访问</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>咨询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>销售</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>经理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息技术</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客服</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>市场</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预算分配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际开销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,6 +147,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -133,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +230,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,6 +282,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -376,7 +474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -417,7 +515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -462,10 +560,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -504,4 +602,195 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A81620-486D-4D5C-ABD0-CA813202B4FE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>55.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C06BBF1-70B5-4368-9D96-49DB12572DB0}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49FA269-1163-45C5-8FDA-AD9F6F855537}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>6500</v>
+      </c>
+      <c r="C2">
+        <v>4300</v>
+      </c>
+      <c r="D2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>16000</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>30000</v>
+      </c>
+      <c r="C4">
+        <v>28000</v>
+      </c>
+      <c r="D4">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>38000</v>
+      </c>
+      <c r="C5">
+        <v>35000</v>
+      </c>
+      <c r="D5">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>52000</v>
+      </c>
+      <c r="C6">
+        <v>50000</v>
+      </c>
+      <c r="D6">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>25000</v>
+      </c>
+      <c r="C7">
+        <v>19000</v>
+      </c>
+      <c r="D7">
+        <v>21000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>